<commit_message>
add filter for table per pertemuan
</commit_message>
<xml_diff>
--- a/upload/rps/1489386205testrps.xlsx
+++ b/upload/rps/1489386205testrps.xlsx
@@ -18,37 +18,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
-    <t xml:space="preserve">Metallic, Ionic, Vanderwalls,Covalent bonding. </t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Atomic structure </t>
-    </r>
-  </si>
-  <si>
     <t>Andi A</t>
   </si>
   <si>
-    <t>Fisika</t>
-  </si>
-  <si>
     <t>PERTEMUAN</t>
   </si>
   <si>
@@ -61,14 +33,23 @@
     <t>MATAKULIAH</t>
   </si>
   <si>
-    <t>Stress &amp; strain curve</t>
+    <t>Kalkulus I</t>
+  </si>
+  <si>
+    <t>Rumus luas persegi</t>
+  </si>
+  <si>
+    <t>Rumus keliling lingkaran</t>
+  </si>
+  <si>
+    <t>Rumus luas segitiga</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,13 +59,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="7"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -131,7 +105,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -441,7 +415,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,16 +428,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -471,41 +445,41 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>2</v>
-      </c>
       <c r="D3" s="4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>